<commit_message>
fix issue with xlo vs x_lo in ecm data
</commit_message>
<xml_diff>
--- a/data/sampling/ic_icpms/ic_icpms_data.xlsx
+++ b/data/sampling/ic_icpms/ic_icpms_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/alhic1901_deep_layering/github/data/sampling/ic_icpms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B77EC2-7FA7-B841-BB6D-94E32A2A6606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2978EA0-D850-324C-A856-5FEF733FCE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10360" yWindow="-21100" windowWidth="18180" windowHeight="21100" xr2:uid="{CFB0DC14-1812-354F-9E14-8529713485B8}"/>
+    <workbookView xWindow="1020" yWindow="760" windowWidth="29220" windowHeight="18880" xr2:uid="{CFB0DC14-1812-354F-9E14-8529713485B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>228_4</t>
   </si>
   <si>
-    <t>ICMPS</t>
-  </si>
-  <si>
     <t>Li</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>stick2</t>
+  </si>
+  <si>
+    <t>ICPMS</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:BD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,136 +653,136 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>38</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>40</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>41</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>44</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>45</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>46</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>47</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>48</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>49</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>50</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>51</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>52</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>53</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>54</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>55</v>
       </c>
-      <c r="BA1" t="s">
-        <v>56</v>
-      </c>
       <c r="BB1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC1" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>59</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>155.083</v>
@@ -1501,7 +1501,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>155.11500000000001</v>
@@ -1642,7 +1642,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>155.14699999999999</v>
@@ -1783,7 +1783,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>155.18549999999999</v>
@@ -1924,7 +1924,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>155.2165</v>
@@ -2065,7 +2065,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C22">
         <v>155.24799999999999</v>
@@ -2206,7 +2206,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C23">
         <v>155.286</v>
@@ -2344,10 +2344,10 @@
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <v>156.8152</v>
@@ -2490,10 +2490,10 @@
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25">
         <v>156.83049389999999</v>
@@ -2636,10 +2636,10 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26">
         <v>156.8429984</v>
@@ -2782,10 +2782,10 @@
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>156.8564025</v>
@@ -2928,10 +2928,10 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>156.8690622</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29">
         <v>156.8829236</v>
@@ -3220,10 +3220,10 @@
     </row>
     <row r="30" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30">
         <v>156.89620719999999</v>
@@ -3366,10 +3366,10 @@
     </row>
     <row r="31" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31">
         <v>156.91009</v>
@@ -3512,10 +3512,10 @@
     </row>
     <row r="32" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32">
         <v>156.92437000000001</v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33">
         <v>156.93795900000001</v>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="34" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34">
         <v>156.95110600000001</v>
@@ -3950,10 +3950,10 @@
     </row>
     <row r="35" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>156.96452500000001</v>
@@ -4096,10 +4096,10 @@
     </row>
     <row r="36" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <v>156.97749899999999</v>
@@ -4242,10 +4242,10 @@
     </row>
     <row r="37" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37">
         <v>156.99092099999999</v>
@@ -4388,10 +4388,10 @@
     </row>
     <row r="38" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38">
         <v>157.00419099999999</v>
@@ -4534,10 +4534,10 @@
     </row>
     <row r="39" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39">
         <v>157.01694800000001</v>
@@ -4680,10 +4680,10 @@
     </row>
     <row r="40" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40">
         <v>157.029854</v>

</xml_diff>